<commit_message>
Consolidating final comments on model and vizs
</commit_message>
<xml_diff>
--- a/xlsx/tehsil_mouzatoshp2022.xlsx
+++ b/xlsx/tehsil_mouzatoshp2022.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb578340\OneDrive - WBG\Documents\WB_FY2023\KPK Population Growth Analysis\KP_Pop_ServiceAccessibility_Project\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4904053-9AC9-4433-B84D-2A5ABA9C3621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33763071-3151-4811-B42B-8A364ECC1F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{B56CC521-9356-4CC0-A5A3-08903D8E1DA9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{B56CC521-9356-4CC0-A5A3-08903D8E1DA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="FuzzyLookup_AddIn_Undo_Sheet" sheetId="4" state="hidden" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="fuzzyjoin_adm3" sheetId="6" r:id="rId4"/>
+    <sheet name="shp2018toshp2022_map" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="10" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2251" uniqueCount="347">
   <si>
     <t xml:space="preserve">Abbottabad </t>
   </si>
@@ -965,18 +967,157 @@
   </si>
   <si>
     <t>khel</t>
+  </si>
+  <si>
+    <t>Chiksar</t>
+  </si>
+  <si>
+    <t>Upper Moma</t>
+  </si>
+  <si>
+    <t>Landi Kota</t>
+  </si>
+  <si>
+    <t>Samar Bagh</t>
+  </si>
+  <si>
+    <t>Matta Khar</t>
+  </si>
+  <si>
+    <t>Matta Sebu</t>
+  </si>
+  <si>
+    <t>Khwazakhel</t>
+  </si>
+  <si>
+    <t>Lower Orak</t>
+  </si>
+  <si>
+    <t>Pindiali</t>
+  </si>
+  <si>
+    <t>Balakot</t>
+  </si>
+  <si>
+    <t>Salarzai T</t>
+  </si>
+  <si>
+    <t>Chagharzai</t>
+  </si>
+  <si>
+    <t>Upper Kurr</t>
+  </si>
+  <si>
+    <t>Martung</t>
+  </si>
+  <si>
+    <t>Pir Baba/</t>
+  </si>
+  <si>
+    <t>Upper Orak</t>
+  </si>
+  <si>
+    <t>Swat Raniz</t>
+  </si>
+  <si>
+    <t>Hassan Khe</t>
+  </si>
+  <si>
+    <t>Dera Ismai</t>
+  </si>
+  <si>
+    <t>Chamla</t>
+  </si>
+  <si>
+    <t>Banda Daud</t>
+  </si>
+  <si>
+    <t>Totalai</t>
+  </si>
+  <si>
+    <t>Lower Kurr</t>
+  </si>
+  <si>
+    <t>Sarai Naur</t>
+  </si>
+  <si>
+    <t>Ambar Utma</t>
+  </si>
+  <si>
+    <t>Central Or</t>
+  </si>
+  <si>
+    <t>Darra Adam</t>
+  </si>
+  <si>
+    <t>Ghulam Kha</t>
+  </si>
+  <si>
+    <t>Central Ku</t>
+  </si>
+  <si>
+    <t>Sam Raniza</t>
+  </si>
+  <si>
+    <t>Lakki Marw</t>
+  </si>
+  <si>
+    <t>Alai</t>
+  </si>
+  <si>
+    <t>Takht E Na</t>
+  </si>
+  <si>
+    <t>Drazanda</t>
+  </si>
+  <si>
+    <t>Serwekai</t>
+  </si>
+  <si>
+    <t>Bar Chamar</t>
+  </si>
+  <si>
+    <t>Kohistan</t>
+  </si>
+  <si>
+    <t>Malakand PA</t>
+  </si>
+  <si>
+    <t>Dera Ismail Khan</t>
+  </si>
+  <si>
+    <t>FR Peshawar</t>
+  </si>
+  <si>
+    <t>FR Kohat</t>
+  </si>
+  <si>
+    <t>FR Bannu</t>
+  </si>
+  <si>
+    <t>FR Dera Ismail Khan</t>
+  </si>
+  <si>
+    <t>FR Lakki Marwat</t>
+  </si>
+  <si>
+    <t>FR Tank</t>
+  </si>
+  <si>
+    <t>FL_pop_EAI%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1008,6 +1149,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1077,7 +1226,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,6 +1254,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1112,7 +1267,94 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Garamond"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Garamond"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1175,6 +1417,13 @@
       </font>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1200,11 +1449,29 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Garamond"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7677,11 +7944,33 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3621D3DF-8EDB-4427-AC56-7571E4C18890}" name="Table2" displayName="Table2" ref="D1:E154" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3621D3DF-8EDB-4427-AC56-7571E4C18890}" name="Table2" displayName="Table2" ref="D1:E154" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="D1:E154" xr:uid="{3621D3DF-8EDB-4427-AC56-7571E4C18890}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AD819141-2E04-46C6-9875-EF5F220633E1}" name="ADM3_NAME" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{1E14DDFE-E7D3-4726-A21B-722C8CF74647}" name="ADM3_CODE" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{AD819141-2E04-46C6-9875-EF5F220633E1}" name="ADM3_NAME" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{1E14DDFE-E7D3-4726-A21B-722C8CF74647}" name="ADM3_CODE" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03E8C0F2-C803-4772-A5BE-02D45993CEF4}" name="Table24" displayName="Table24" ref="A1:A154" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4">
+  <autoFilter ref="A1:A154" xr:uid="{03E8C0F2-C803-4772-A5BE-02D45993CEF4}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{EDD78F6B-DE86-4592-8369-7A866423AD11}" name="ADM3_NAME" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6613B7C9-0632-468D-866B-E46A3A269960}" name="Table5" displayName="Table5" ref="F1:H117" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="F1:H117" xr:uid="{6613B7C9-0632-468D-866B-E46A3A269960}"/>
+  <tableColumns count="3">
+    <tableColumn id="5" xr3:uid="{255F324C-FAF2-495E-8166-76E37E725497}" name="ADM2_NAME"/>
+    <tableColumn id="6" xr3:uid="{4202DE8E-D890-4A48-98E8-B67FC0DD45F8}" name="ADM3_NAME"/>
+    <tableColumn id="7" xr3:uid="{DF4D366F-0CD6-4DCB-AF2E-7CAC7FDBFAEF}" name="FL_pop_EAI%" dataDxfId="1" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7987,7 +8276,7 @@
   <dimension ref="A1:P154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11500,8 +11789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A9B521-AF8A-4256-8083-50F669EBB9EF}">
   <dimension ref="A1:X155"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24489,7 +24778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F8DFC3-EEF6-40B6-AE04-C995994FDF6A}">
   <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -26430,4 +26719,3837 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401B85F2-422D-4498-867A-3C75B350C4F4}">
+  <dimension ref="A1:H154"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="26">
+        <v>8.4279486546003096E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>332</v>
+      </c>
+      <c r="H3" s="26">
+        <v>2.5234471954996059E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="26">
+        <v>3.5300274470223829E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G5" t="s">
+        <v>325</v>
+      </c>
+      <c r="H5" s="26">
+        <v>2.2351631203187754E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="26">
+        <v>3.0159907400122438E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" t="s">
+        <v>281</v>
+      </c>
+      <c r="H7" s="26">
+        <v>2.7735480138966688E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>310</v>
+      </c>
+      <c r="H8" s="26">
+        <v>1.9473996956734815E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>321</v>
+      </c>
+      <c r="H9" s="26">
+        <v>3.528518421418101E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="26">
+        <v>5.4993554518878969E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" t="s">
+        <v>336</v>
+      </c>
+      <c r="H11" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" t="s">
+        <v>200</v>
+      </c>
+      <c r="H12" s="26">
+        <v>4.0095705630711312E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H13" s="26">
+        <v>4.404068276641921E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" t="s">
+        <v>291</v>
+      </c>
+      <c r="G14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H14" s="26">
+        <v>1.6335232496571409E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="26">
+        <v>5.2190152951596613E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="26">
+        <v>1.4344217833188516E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" t="s">
+        <v>344</v>
+      </c>
+      <c r="G17" t="s">
+        <v>219</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F18" t="s">
+        <v>272</v>
+      </c>
+      <c r="G18" t="s">
+        <v>271</v>
+      </c>
+      <c r="H18" s="26">
+        <v>1.0317017634070456E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>267</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="26">
+        <v>5.8066192657883666E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>214</v>
+      </c>
+      <c r="G20" t="s">
+        <v>329</v>
+      </c>
+      <c r="H20" s="26">
+        <v>8.2389083111011292E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" t="s">
+        <v>257</v>
+      </c>
+      <c r="G21" t="s">
+        <v>326</v>
+      </c>
+      <c r="H21" s="26">
+        <v>1.6188129785937346E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
+        <v>183</v>
+      </c>
+      <c r="G22" t="s">
+        <v>312</v>
+      </c>
+      <c r="H22" s="26">
+        <v>1.6858688474822306E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" t="s">
+        <v>183</v>
+      </c>
+      <c r="G23" t="s">
+        <v>320</v>
+      </c>
+      <c r="H23" s="26">
+        <v>4.2976337257862083E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="26">
+        <v>7.798391858276112E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="26">
+        <v>1.0393084515879693E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" t="s">
+        <v>267</v>
+      </c>
+      <c r="G26" t="s">
+        <v>301</v>
+      </c>
+      <c r="H26" s="26">
+        <v>2.7096715750456841E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F27" t="s">
+        <v>185</v>
+      </c>
+      <c r="G27" t="s">
+        <v>185</v>
+      </c>
+      <c r="H27" s="26">
+        <v>5.2904433633162726E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F28" t="s">
+        <v>183</v>
+      </c>
+      <c r="G28" t="s">
+        <v>182</v>
+      </c>
+      <c r="H28" s="26">
+        <v>5.0037365765034819E-5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F29" t="s">
+        <v>339</v>
+      </c>
+      <c r="G29" t="s">
+        <v>193</v>
+      </c>
+      <c r="H29" s="26">
+        <v>2.6149702656153361E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F30" t="s">
+        <v>341</v>
+      </c>
+      <c r="G30" t="s">
+        <v>327</v>
+      </c>
+      <c r="H30" s="26">
+        <v>9.1874801034898807E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F31" t="s">
+        <v>337</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="26">
+        <v>6.4524507441887681E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G32" t="s">
+        <v>244</v>
+      </c>
+      <c r="H32" s="26">
+        <v>1.3242897030416484E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H33" s="26">
+        <v>4.5511471342504325E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F34" t="s">
+        <v>291</v>
+      </c>
+      <c r="G34" t="s">
+        <v>292</v>
+      </c>
+      <c r="H34" s="26">
+        <v>2.7301063822618671E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F36" t="s">
+        <v>245</v>
+      </c>
+      <c r="G36" t="s">
+        <v>246</v>
+      </c>
+      <c r="H36" s="26">
+        <v>1.0963261688418198E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" t="s">
+        <v>343</v>
+      </c>
+      <c r="G37" t="s">
+        <v>334</v>
+      </c>
+      <c r="H37" s="26">
+        <v>8.3085984971307333E-8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" t="s">
+        <v>183</v>
+      </c>
+      <c r="G38" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="26">
+        <v>9.5334124013108558E-5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>245</v>
+      </c>
+      <c r="G39" t="s">
+        <v>247</v>
+      </c>
+      <c r="H39" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" s="26">
+        <v>1.2852890377049848E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" t="s">
+        <v>245</v>
+      </c>
+      <c r="G41" t="s">
+        <v>328</v>
+      </c>
+      <c r="H41" s="26">
+        <v>9.1012672257199878E-6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" t="s">
+        <v>236</v>
+      </c>
+      <c r="G42" t="s">
+        <v>238</v>
+      </c>
+      <c r="H42" s="26">
+        <v>3.7365288127740175E-6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" t="s">
+        <v>45</v>
+      </c>
+      <c r="G43" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" s="26">
+        <v>7.1004531336510992E-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F44" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" s="26">
+        <v>6.7888003093236331E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" t="s">
+        <v>340</v>
+      </c>
+      <c r="G45" t="s">
+        <v>318</v>
+      </c>
+      <c r="H45" s="26">
+        <v>4.6067171053971244E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F46" t="s">
+        <v>257</v>
+      </c>
+      <c r="G46" t="s">
+        <v>258</v>
+      </c>
+      <c r="H46" s="26">
+        <v>8.9732852887092488E-6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" t="s">
+        <v>201</v>
+      </c>
+      <c r="G47" t="s">
+        <v>202</v>
+      </c>
+      <c r="H47" s="26">
+        <v>1.8402480948462463E-5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F48" t="s">
+        <v>345</v>
+      </c>
+      <c r="G48" t="s">
+        <v>286</v>
+      </c>
+      <c r="H48" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F49" t="s">
+        <v>120</v>
+      </c>
+      <c r="G49" t="s">
+        <v>55</v>
+      </c>
+      <c r="H49" s="26">
+        <v>5.9483313332917818E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" t="s">
+        <v>120</v>
+      </c>
+      <c r="G50" t="s">
+        <v>282</v>
+      </c>
+      <c r="H50" s="26">
+        <v>2.7562644689105432E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F51" t="s">
+        <v>291</v>
+      </c>
+      <c r="G51" t="s">
+        <v>293</v>
+      </c>
+      <c r="H51" s="26">
+        <v>3.9566123137140061E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" t="s">
+        <v>58</v>
+      </c>
+      <c r="G52" t="s">
+        <v>58</v>
+      </c>
+      <c r="H52" s="26">
+        <v>1.5223642251383361E-6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F53" t="s">
+        <v>80</v>
+      </c>
+      <c r="G53" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" s="26">
+        <v>4.6963087418143541E-6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F54" t="s">
+        <v>172</v>
+      </c>
+      <c r="G54" t="s">
+        <v>174</v>
+      </c>
+      <c r="H54" s="26">
+        <v>1.0972726213917836E-5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" t="s">
+        <v>120</v>
+      </c>
+      <c r="G55" t="s">
+        <v>307</v>
+      </c>
+      <c r="H55" s="26">
+        <v>2.4254358966350044E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
+        <v>205</v>
+      </c>
+      <c r="G56" t="s">
+        <v>205</v>
+      </c>
+      <c r="H56" s="26">
+        <v>1.7803648643190942E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F57" t="s">
+        <v>339</v>
+      </c>
+      <c r="G57" t="s">
+        <v>194</v>
+      </c>
+      <c r="H57" s="26">
+        <v>5.1118108746740893E-6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F58" t="s">
+        <v>205</v>
+      </c>
+      <c r="G58" t="s">
+        <v>66</v>
+      </c>
+      <c r="H58" s="26">
+        <v>6.0350594472979887E-6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F59" t="s">
+        <v>272</v>
+      </c>
+      <c r="G59" t="s">
+        <v>273</v>
+      </c>
+      <c r="H59" s="26">
+        <v>4.1120242444649298E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F60" t="s">
+        <v>119</v>
+      </c>
+      <c r="G60" t="s">
+        <v>280</v>
+      </c>
+      <c r="H60" s="26">
+        <v>7.6765446364029642E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" t="s">
+        <v>217</v>
+      </c>
+      <c r="G61" t="s">
+        <v>331</v>
+      </c>
+      <c r="H61" s="26">
+        <v>5.0227905174926858E-6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F62" t="s">
+        <v>201</v>
+      </c>
+      <c r="G62" t="s">
+        <v>303</v>
+      </c>
+      <c r="H62" s="26">
+        <v>1.271608375439396E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F63" t="s">
+        <v>214</v>
+      </c>
+      <c r="G63" t="s">
+        <v>323</v>
+      </c>
+      <c r="H63" s="26">
+        <v>2.8056802090876943E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F64" t="s">
+        <v>257</v>
+      </c>
+      <c r="G64" t="s">
+        <v>308</v>
+      </c>
+      <c r="H64" s="26">
+        <v>2.3416476876623261E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F65" t="s">
+        <v>272</v>
+      </c>
+      <c r="G65" t="s">
+        <v>274</v>
+      </c>
+      <c r="H65" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F66" t="s">
+        <v>172</v>
+      </c>
+      <c r="G66" t="s">
+        <v>175</v>
+      </c>
+      <c r="H66" s="26">
+        <v>5.7673285063573884E-8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F67" t="s">
+        <v>79</v>
+      </c>
+      <c r="G67" t="s">
+        <v>79</v>
+      </c>
+      <c r="H67" s="26">
+        <v>8.8259153967178684E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F68" t="s">
+        <v>80</v>
+      </c>
+      <c r="G68" t="s">
+        <v>80</v>
+      </c>
+      <c r="H68" s="26">
+        <v>2.3906816161356429E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F69" t="s">
+        <v>267</v>
+      </c>
+      <c r="G69" t="s">
+        <v>314</v>
+      </c>
+      <c r="H69" s="26">
+        <v>9.6787366099330478E-5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F70" t="s">
+        <v>185</v>
+      </c>
+      <c r="G70" t="s">
+        <v>189</v>
+      </c>
+      <c r="H70" s="26">
+        <v>2.1642437409737261E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F71" t="s">
+        <v>120</v>
+      </c>
+      <c r="G71" t="s">
+        <v>305</v>
+      </c>
+      <c r="H71" s="26">
+        <v>4.9175660186531625E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F72" t="s">
+        <v>120</v>
+      </c>
+      <c r="G72" t="s">
+        <v>306</v>
+      </c>
+      <c r="H72" s="26">
+        <v>2.4387127481237525E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="F73" t="s">
+        <v>245</v>
+      </c>
+      <c r="G73" t="s">
+        <v>249</v>
+      </c>
+      <c r="H73" s="26">
+        <v>6.8855516731707806E-6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F74" t="s">
+        <v>245</v>
+      </c>
+      <c r="G74" t="s">
+        <v>250</v>
+      </c>
+      <c r="H74" s="26">
+        <v>4.1758043223798071E-6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F75" t="s">
+        <v>172</v>
+      </c>
+      <c r="G75" t="s">
+        <v>176</v>
+      </c>
+      <c r="H75" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F76" t="s">
+        <v>255</v>
+      </c>
+      <c r="G76" t="s">
+        <v>255</v>
+      </c>
+      <c r="H76" s="26">
+        <v>1.4548639266513995E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F77" t="s">
+        <v>79</v>
+      </c>
+      <c r="G77" t="s">
+        <v>91</v>
+      </c>
+      <c r="H77" s="26">
+        <v>1.8022787179572671E-4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F78" t="s">
+        <v>255</v>
+      </c>
+      <c r="G78" t="s">
+        <v>92</v>
+      </c>
+      <c r="H78" s="26">
+        <v>4.6917003879934474E-4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F79" t="s">
+        <v>339</v>
+      </c>
+      <c r="G79" t="s">
+        <v>195</v>
+      </c>
+      <c r="H79" s="26">
+        <v>4.6071336726762833E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="F80" t="s">
+        <v>337</v>
+      </c>
+      <c r="G80" t="s">
+        <v>94</v>
+      </c>
+      <c r="H80" s="26">
+        <v>2.1061574705569206E-4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F81" t="s">
+        <v>337</v>
+      </c>
+      <c r="G81" t="s">
+        <v>96</v>
+      </c>
+      <c r="H81" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F82" t="s">
+        <v>262</v>
+      </c>
+      <c r="G82" t="s">
+        <v>262</v>
+      </c>
+      <c r="H82" s="26">
+        <v>6.8319235915313646E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F83" t="s">
+        <v>236</v>
+      </c>
+      <c r="G83" t="s">
+        <v>309</v>
+      </c>
+      <c r="H83" s="26">
+        <v>2.0549513224376361E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F84" t="s">
+        <v>183</v>
+      </c>
+      <c r="G84" t="s">
+        <v>315</v>
+      </c>
+      <c r="H84" s="26">
+        <v>5.6205318071558236E-5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F85" t="s">
+        <v>236</v>
+      </c>
+      <c r="G85" t="s">
+        <v>241</v>
+      </c>
+      <c r="H85" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F86" t="s">
+        <v>267</v>
+      </c>
+      <c r="G86" t="s">
+        <v>101</v>
+      </c>
+      <c r="H86" s="26">
+        <v>3.9211027416015301E-4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F87" t="s">
+        <v>245</v>
+      </c>
+      <c r="G87" t="s">
+        <v>251</v>
+      </c>
+      <c r="H87" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F88" t="s">
+        <v>236</v>
+      </c>
+      <c r="G88" t="s">
+        <v>242</v>
+      </c>
+      <c r="H88" s="26">
+        <v>1.3450318992235812E-5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A89" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F89" t="s">
+        <v>172</v>
+      </c>
+      <c r="G89" t="s">
+        <v>311</v>
+      </c>
+      <c r="H89" s="26">
+        <v>1.9416321548088822E-4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F90" t="s">
+        <v>338</v>
+      </c>
+      <c r="G90" t="s">
+        <v>330</v>
+      </c>
+      <c r="H90" s="26">
+        <v>6.6399417046860326E-6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F91" t="s">
+        <v>222</v>
+      </c>
+      <c r="G91" t="s">
+        <v>304</v>
+      </c>
+      <c r="H91" s="26">
+        <v>6.1002578476629051E-4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F92" t="s">
+        <v>217</v>
+      </c>
+      <c r="G92" t="s">
+        <v>324</v>
+      </c>
+      <c r="H92" s="26">
+        <v>2.5454080422313591E-5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F93" t="s">
+        <v>272</v>
+      </c>
+      <c r="G93" t="s">
+        <v>275</v>
+      </c>
+      <c r="H93" s="26">
+        <v>3.0834960151569861E-8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F94" t="s">
+        <v>272</v>
+      </c>
+      <c r="G94" t="s">
+        <v>335</v>
+      </c>
+      <c r="H94" s="26">
+        <v>1.9959046431807505E-8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F95" t="s">
+        <v>245</v>
+      </c>
+      <c r="G95" t="s">
+        <v>252</v>
+      </c>
+      <c r="H95" s="26">
+        <v>1.5335387809345196E-4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F96" t="s">
+        <v>245</v>
+      </c>
+      <c r="G96" t="s">
+        <v>253</v>
+      </c>
+      <c r="H96" s="26">
+        <v>3.4162320763967882E-8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F97" t="s">
+        <v>119</v>
+      </c>
+      <c r="G97" t="s">
+        <v>119</v>
+      </c>
+      <c r="H97" s="26">
+        <v>7.2158514511182475E-6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F98" t="s">
+        <v>338</v>
+      </c>
+      <c r="G98" t="s">
+        <v>317</v>
+      </c>
+      <c r="H98" s="26">
+        <v>4.6165768657092907E-5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F99" t="s">
+        <v>80</v>
+      </c>
+      <c r="G99" t="s">
+        <v>232</v>
+      </c>
+      <c r="H99" s="26">
+        <v>1.2089471745314076E-5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F100" t="s">
+        <v>58</v>
+      </c>
+      <c r="G100" t="s">
+        <v>333</v>
+      </c>
+      <c r="H100" s="26">
+        <v>3.846843370313005E-7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F101" t="s">
+        <v>45</v>
+      </c>
+      <c r="G101" t="s">
+        <v>197</v>
+      </c>
+      <c r="H101" s="26">
+        <v>2.4598878915963857E-5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="F102" t="s">
+        <v>25</v>
+      </c>
+      <c r="G102" t="s">
+        <v>124</v>
+      </c>
+      <c r="H102" s="26">
+        <v>2.0611971961472501E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F103" t="s">
+        <v>125</v>
+      </c>
+      <c r="G103" t="s">
+        <v>125</v>
+      </c>
+      <c r="H103" s="26">
+        <v>4.9560589557760846E-7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F104" t="s">
+        <v>272</v>
+      </c>
+      <c r="G104" t="s">
+        <v>277</v>
+      </c>
+      <c r="H104" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F105" t="s">
+        <v>222</v>
+      </c>
+      <c r="G105" t="s">
+        <v>227</v>
+      </c>
+      <c r="H105" s="26">
+        <v>2.6222760849559611E-4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F106" t="s">
+        <v>272</v>
+      </c>
+      <c r="G106" t="s">
+        <v>278</v>
+      </c>
+      <c r="H106" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A107" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F107" t="s">
+        <v>119</v>
+      </c>
+      <c r="G107" t="s">
+        <v>130</v>
+      </c>
+      <c r="H107" s="26">
+        <v>5.0223820436918619E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F108" t="s">
+        <v>288</v>
+      </c>
+      <c r="G108" t="s">
+        <v>288</v>
+      </c>
+      <c r="H108" s="26">
+        <v>1.4942570235631151E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="F109" t="s">
+        <v>183</v>
+      </c>
+      <c r="G109" t="s">
+        <v>322</v>
+      </c>
+      <c r="H109" s="26">
+        <v>2.8488609724669997E-5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F110" t="s">
+        <v>214</v>
+      </c>
+      <c r="G110" t="s">
+        <v>313</v>
+      </c>
+      <c r="H110" s="26">
+        <v>1.0477301881350609E-4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F111" t="s">
+        <v>236</v>
+      </c>
+      <c r="G111" t="s">
+        <v>302</v>
+      </c>
+      <c r="H111" s="26">
+        <v>1.6444793796865833E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F112" t="s">
+        <v>257</v>
+      </c>
+      <c r="G112" t="s">
+        <v>316</v>
+      </c>
+      <c r="H112" s="26">
+        <v>4.6337151925197988E-5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F113" t="s">
+        <v>172</v>
+      </c>
+      <c r="G113" t="s">
+        <v>178</v>
+      </c>
+      <c r="H113" s="26">
+        <v>4.3930321481960283E-5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F114" t="s">
+        <v>272</v>
+      </c>
+      <c r="G114" t="s">
+        <v>279</v>
+      </c>
+      <c r="H114" s="26">
+        <v>3.4524285007145288E-5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A115" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F115" t="s">
+        <v>291</v>
+      </c>
+      <c r="G115" t="s">
+        <v>296</v>
+      </c>
+      <c r="H115" s="26">
+        <v>9.8018242020467576E-4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A116" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="F116" t="s">
+        <v>342</v>
+      </c>
+      <c r="G116" t="s">
+        <v>181</v>
+      </c>
+      <c r="H116" s="26">
+        <v>5.9725825881480801E-6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A117" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F117" t="s">
+        <v>236</v>
+      </c>
+      <c r="G117" t="s">
+        <v>243</v>
+      </c>
+      <c r="H117" s="26">
+        <v>3.0636495853792029E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A119" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A124" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A125" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A126" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A127" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A128" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" s="22" t="s">
+        <v>297</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:H117">
+    <sortCondition ref="G2:G117"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B1F091C-27FA-4CF9-BAEF-F043E69F9E4D}">
+  <dimension ref="A1:E117"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>346</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="27">
+        <v>8.4279486546003096E-5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C3" s="27">
+        <v>2.5234471954996102E-6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0.91790048309382533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3.5300274470223799E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="27">
+        <v>2.2351631203187801E-5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="27">
+        <v>3.0159907400122401E-5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7">
+        <v>2.7735480138966701E-3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E7" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>310</v>
+      </c>
+      <c r="C8">
+        <v>1.9473996956734799E-4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.97087378640776689</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="27">
+        <v>3.5285184214180997E-5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.94285714285714284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="27">
+        <v>5.4993554518879003E-6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" t="s">
+        <v>336</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0.80522875816993467</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12">
+        <v>4.0095705630711301E-4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E12" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C13" s="27">
+        <v>4.4040682766419201E-6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C14">
+        <v>1.63352324965714E-3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="27">
+        <v>5.2190152951596599E-5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>1.4344217833188501E-3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>344</v>
+      </c>
+      <c r="B17" t="s">
+        <v>219</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>219</v>
+      </c>
+      <c r="E17" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>272</v>
+      </c>
+      <c r="B18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C18" s="27">
+        <v>1.03170176340705E-5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>271</v>
+      </c>
+      <c r="E18" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>5.8066192657883699E-4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" t="s">
+        <v>329</v>
+      </c>
+      <c r="C20" s="27">
+        <v>8.2389083111011292E-6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0.78691594254321739</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>257</v>
+      </c>
+      <c r="B21" t="s">
+        <v>326</v>
+      </c>
+      <c r="C21" s="27">
+        <v>1.6188129785937299E-5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="24">
+        <v>0.78691594254321739</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" t="s">
+        <v>312</v>
+      </c>
+      <c r="C22">
+        <v>1.6858688474822301E-4</v>
+      </c>
+      <c r="E22" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" t="s">
+        <v>320</v>
+      </c>
+      <c r="C23" s="27">
+        <v>4.2976337257862103E-5</v>
+      </c>
+      <c r="E23" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="27">
+        <v>7.7983918582761104E-6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>1.0393084515879699E-4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>267</v>
+      </c>
+      <c r="B26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26">
+        <v>2.7096715750456802E-3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>268</v>
+      </c>
+      <c r="E26" s="24">
+        <v>0.89626360019790874</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27">
+        <v>5.29044336331627E-3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>185</v>
+      </c>
+      <c r="E27" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="27">
+        <v>5.0037365765034799E-5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>339</v>
+      </c>
+      <c r="B29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="27">
+        <v>2.6149702656153399E-5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>341</v>
+      </c>
+      <c r="B30" t="s">
+        <v>327</v>
+      </c>
+      <c r="C30" s="27">
+        <v>9.1874801034898807E-6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>207</v>
+      </c>
+      <c r="E30" s="24">
+        <v>0.9538461538461539</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>337</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>6.4524507441887698E-3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>245</v>
+      </c>
+      <c r="B32" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32">
+        <v>1.32428970304165E-4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>244</v>
+      </c>
+      <c r="E32" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>339</v>
+      </c>
+      <c r="B33" t="s">
+        <v>319</v>
+      </c>
+      <c r="C33" s="27">
+        <v>4.5511471342504298E-5</v>
+      </c>
+      <c r="E33" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>291</v>
+      </c>
+      <c r="B34" t="s">
+        <v>292</v>
+      </c>
+      <c r="C34">
+        <v>2.7301063822618701E-3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>292</v>
+      </c>
+      <c r="E34" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>245</v>
+      </c>
+      <c r="B36" t="s">
+        <v>246</v>
+      </c>
+      <c r="C36" s="27">
+        <v>1.09632616884182E-5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>246</v>
+      </c>
+      <c r="E36" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>343</v>
+      </c>
+      <c r="B37" t="s">
+        <v>334</v>
+      </c>
+      <c r="C37" s="27">
+        <v>8.3085984971307294E-8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>196</v>
+      </c>
+      <c r="E37" s="24">
+        <v>0.9051767918727287</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="27">
+        <v>9.5334124013108599E-5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>245</v>
+      </c>
+      <c r="B39" t="s">
+        <v>247</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>247</v>
+      </c>
+      <c r="E39" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40">
+        <v>1.28528903770498E-3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>245</v>
+      </c>
+      <c r="B41" t="s">
+        <v>328</v>
+      </c>
+      <c r="C41" s="27">
+        <v>9.1012672257199895E-6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="24">
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>236</v>
+      </c>
+      <c r="B42" t="s">
+        <v>238</v>
+      </c>
+      <c r="C42" s="27">
+        <v>3.73652881277402E-6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>238</v>
+      </c>
+      <c r="E42" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="27">
+        <v>7.1004531336511E-6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E43" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="27">
+        <v>6.7888003093236304E-5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>340</v>
+      </c>
+      <c r="B45" t="s">
+        <v>318</v>
+      </c>
+      <c r="C45" s="27">
+        <v>4.6067171053971197E-5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>266</v>
+      </c>
+      <c r="E45" s="24">
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>257</v>
+      </c>
+      <c r="B46" t="s">
+        <v>258</v>
+      </c>
+      <c r="C46" s="27">
+        <v>8.9732852887092505E-6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>258</v>
+      </c>
+      <c r="E46" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>201</v>
+      </c>
+      <c r="B47" t="s">
+        <v>202</v>
+      </c>
+      <c r="C47" s="27">
+        <v>1.8402480948462501E-5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>202</v>
+      </c>
+      <c r="E47" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>345</v>
+      </c>
+      <c r="B48" t="s">
+        <v>286</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>286</v>
+      </c>
+      <c r="E48" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="27">
+        <v>5.9483313332917798E-5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E49" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" t="s">
+        <v>282</v>
+      </c>
+      <c r="C50">
+        <v>2.7562644689105402E-3</v>
+      </c>
+      <c r="D50" t="s">
+        <v>282</v>
+      </c>
+      <c r="E50" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>291</v>
+      </c>
+      <c r="B51" t="s">
+        <v>293</v>
+      </c>
+      <c r="C51">
+        <v>3.9566123137140096E-3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>293</v>
+      </c>
+      <c r="E51" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="27">
+        <v>1.5223642251383399E-6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="27">
+        <v>4.6963087418143498E-6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>59</v>
+      </c>
+      <c r="E53" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" t="s">
+        <v>174</v>
+      </c>
+      <c r="C54" s="27">
+        <v>1.09727262139178E-5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" t="s">
+        <v>307</v>
+      </c>
+      <c r="C55">
+        <v>2.4254358966350001E-4</v>
+      </c>
+      <c r="E55" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56" t="s">
+        <v>205</v>
+      </c>
+      <c r="C56">
+        <v>1.7803648643190901E-4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>205</v>
+      </c>
+      <c r="E56" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>339</v>
+      </c>
+      <c r="B57" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="27">
+        <v>5.1118108746740902E-6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>205</v>
+      </c>
+      <c r="B58" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="27">
+        <v>6.0350594472979904E-6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>272</v>
+      </c>
+      <c r="B59" t="s">
+        <v>273</v>
+      </c>
+      <c r="C59">
+        <v>4.1120242444649298E-3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>273</v>
+      </c>
+      <c r="E59" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" t="s">
+        <v>280</v>
+      </c>
+      <c r="C60" s="27">
+        <v>7.6765446364029602E-5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>280</v>
+      </c>
+      <c r="E60" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>217</v>
+      </c>
+      <c r="B61" t="s">
+        <v>331</v>
+      </c>
+      <c r="C61" s="27">
+        <v>5.0227905174926901E-6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>217</v>
+      </c>
+      <c r="E61" s="24">
+        <v>0.91222144646330328</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" t="s">
+        <v>303</v>
+      </c>
+      <c r="C62">
+        <v>1.2716083754394001E-3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>203</v>
+      </c>
+      <c r="E62" s="24">
+        <v>0.95719302558715791</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>214</v>
+      </c>
+      <c r="B63" t="s">
+        <v>323</v>
+      </c>
+      <c r="C63" s="27">
+        <v>2.8056802090876899E-5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>215</v>
+      </c>
+      <c r="E63" s="24">
+        <v>0.90341032957659839</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>257</v>
+      </c>
+      <c r="B64" t="s">
+        <v>308</v>
+      </c>
+      <c r="C64">
+        <v>2.3416476876623299E-4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>215</v>
+      </c>
+      <c r="E64" s="24">
+        <v>0.46153846153846156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>272</v>
+      </c>
+      <c r="B65" t="s">
+        <v>274</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>274</v>
+      </c>
+      <c r="E65" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>172</v>
+      </c>
+      <c r="B66" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" s="27">
+        <v>5.7673285063573897E-8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>175</v>
+      </c>
+      <c r="E66" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="27">
+        <v>8.8259153967178698E-5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>79</v>
+      </c>
+      <c r="E67" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="27">
+        <v>2.3906816161356398E-5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>80</v>
+      </c>
+      <c r="E68" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>267</v>
+      </c>
+      <c r="B69" t="s">
+        <v>314</v>
+      </c>
+      <c r="C69" s="27">
+        <v>9.6787366099330505E-5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>270</v>
+      </c>
+      <c r="E69" s="24">
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>185</v>
+      </c>
+      <c r="B70" t="s">
+        <v>189</v>
+      </c>
+      <c r="C70">
+        <v>2.16424374097373E-3</v>
+      </c>
+      <c r="D70" t="s">
+        <v>189</v>
+      </c>
+      <c r="E70" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" t="s">
+        <v>305</v>
+      </c>
+      <c r="C71">
+        <v>4.9175660186531603E-4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>174</v>
+      </c>
+      <c r="E71" s="24">
+        <v>0.91111111111111109</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" t="s">
+        <v>306</v>
+      </c>
+      <c r="C72">
+        <v>2.43871274812375E-4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>284</v>
+      </c>
+      <c r="E72" s="24">
+        <v>0.41269841269841268</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>245</v>
+      </c>
+      <c r="B73" t="s">
+        <v>249</v>
+      </c>
+      <c r="C73" s="27">
+        <v>6.8855516731707797E-6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>249</v>
+      </c>
+      <c r="E73" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>245</v>
+      </c>
+      <c r="B74" t="s">
+        <v>250</v>
+      </c>
+      <c r="C74" s="27">
+        <v>4.1758043223798097E-6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>250</v>
+      </c>
+      <c r="E74" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
+        <v>176</v>
+      </c>
+      <c r="E75" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>255</v>
+      </c>
+      <c r="B76" t="s">
+        <v>255</v>
+      </c>
+      <c r="C76">
+        <v>1.4548639266514E-3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>255</v>
+      </c>
+      <c r="E76" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77">
+        <v>1.8022787179572701E-4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>91</v>
+      </c>
+      <c r="E77" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>255</v>
+      </c>
+      <c r="B78" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78">
+        <v>4.6917003879934501E-4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>92</v>
+      </c>
+      <c r="E78" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>339</v>
+      </c>
+      <c r="B79" t="s">
+        <v>195</v>
+      </c>
+      <c r="C79" s="27">
+        <v>4.6071336726762799E-5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>195</v>
+      </c>
+      <c r="E79" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>337</v>
+      </c>
+      <c r="B80" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80">
+        <v>2.1061574705569201E-4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>94</v>
+      </c>
+      <c r="E80" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>337</v>
+      </c>
+      <c r="B81" t="s">
+        <v>96</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>262</v>
+      </c>
+      <c r="B82" t="s">
+        <v>262</v>
+      </c>
+      <c r="C82" s="27">
+        <v>6.8319235915313605E-5</v>
+      </c>
+      <c r="E82" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>236</v>
+      </c>
+      <c r="B83" t="s">
+        <v>309</v>
+      </c>
+      <c r="C83">
+        <v>2.0549513224376399E-4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>240</v>
+      </c>
+      <c r="E83" s="24">
+        <v>0.95767628767520652</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>183</v>
+      </c>
+      <c r="B84" t="s">
+        <v>315</v>
+      </c>
+      <c r="C84" s="27">
+        <v>5.6205318071558202E-5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>200</v>
+      </c>
+      <c r="E84" s="24">
+        <v>0.80522875816993467</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>236</v>
+      </c>
+      <c r="B85" t="s">
+        <v>241</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
+        <v>241</v>
+      </c>
+      <c r="E85" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>267</v>
+      </c>
+      <c r="B86" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86">
+        <v>3.9211027416015301E-4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>101</v>
+      </c>
+      <c r="E86" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>245</v>
+      </c>
+      <c r="B87" t="s">
+        <v>251</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>251</v>
+      </c>
+      <c r="E87" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>236</v>
+      </c>
+      <c r="B88" t="s">
+        <v>242</v>
+      </c>
+      <c r="C88" s="27">
+        <v>1.34503189922358E-5</v>
+      </c>
+      <c r="D88" t="s">
+        <v>242</v>
+      </c>
+      <c r="E88" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>172</v>
+      </c>
+      <c r="B89" t="s">
+        <v>311</v>
+      </c>
+      <c r="C89">
+        <v>1.9416321548088801E-4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>177</v>
+      </c>
+      <c r="E89" s="24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>338</v>
+      </c>
+      <c r="B90" t="s">
+        <v>330</v>
+      </c>
+      <c r="C90" s="27">
+        <v>6.63994170468603E-6</v>
+      </c>
+      <c r="E90" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91" t="s">
+        <v>304</v>
+      </c>
+      <c r="C91">
+        <v>6.1002578476629095E-4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E91" s="24">
+        <v>0.97087378640776689</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>217</v>
+      </c>
+      <c r="B92" t="s">
+        <v>324</v>
+      </c>
+      <c r="C92" s="27">
+        <v>2.5454080422313602E-5</v>
+      </c>
+      <c r="D92" t="s">
+        <v>218</v>
+      </c>
+      <c r="E92" s="24">
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>272</v>
+      </c>
+      <c r="B93" t="s">
+        <v>275</v>
+      </c>
+      <c r="C93" s="27">
+        <v>3.08349601515699E-8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>275</v>
+      </c>
+      <c r="E93" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>272</v>
+      </c>
+      <c r="B94" t="s">
+        <v>335</v>
+      </c>
+      <c r="C94" s="27">
+        <v>1.9959046431807498E-8</v>
+      </c>
+      <c r="D94" t="s">
+        <v>276</v>
+      </c>
+      <c r="E94" s="24">
+        <v>0.95767628767520652</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>245</v>
+      </c>
+      <c r="B95" t="s">
+        <v>252</v>
+      </c>
+      <c r="C95">
+        <v>1.5335387809345199E-4</v>
+      </c>
+      <c r="D95" t="s">
+        <v>252</v>
+      </c>
+      <c r="E95" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>245</v>
+      </c>
+      <c r="B96" t="s">
+        <v>253</v>
+      </c>
+      <c r="C96" s="27">
+        <v>3.4162320763967901E-8</v>
+      </c>
+      <c r="D96" t="s">
+        <v>253</v>
+      </c>
+      <c r="E96" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>119</v>
+      </c>
+      <c r="B97" t="s">
+        <v>119</v>
+      </c>
+      <c r="C97" s="27">
+        <v>7.21585145111825E-6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>119</v>
+      </c>
+      <c r="E97" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>338</v>
+      </c>
+      <c r="B98" t="s">
+        <v>317</v>
+      </c>
+      <c r="C98" s="27">
+        <v>4.61657686570929E-5</v>
+      </c>
+      <c r="E98" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>80</v>
+      </c>
+      <c r="B99" t="s">
+        <v>232</v>
+      </c>
+      <c r="C99" s="27">
+        <v>1.20894717453141E-5</v>
+      </c>
+      <c r="D99" t="s">
+        <v>232</v>
+      </c>
+      <c r="E99" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>58</v>
+      </c>
+      <c r="B100" t="s">
+        <v>333</v>
+      </c>
+      <c r="C100" s="27">
+        <v>3.8468433703130002E-7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>199</v>
+      </c>
+      <c r="E100" s="24">
+        <v>0.60902255639097747</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>45</v>
+      </c>
+      <c r="B101" t="s">
+        <v>197</v>
+      </c>
+      <c r="C101" s="27">
+        <v>2.4598878915963901E-5</v>
+      </c>
+      <c r="D101" t="s">
+        <v>197</v>
+      </c>
+      <c r="E101" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>25</v>
+      </c>
+      <c r="B102" t="s">
+        <v>124</v>
+      </c>
+      <c r="C102">
+        <v>2.0611971961472501E-4</v>
+      </c>
+      <c r="D102" t="s">
+        <v>124</v>
+      </c>
+      <c r="E102" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>125</v>
+      </c>
+      <c r="B103" t="s">
+        <v>125</v>
+      </c>
+      <c r="C103" s="27">
+        <v>4.9560589557760803E-7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E103" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>272</v>
+      </c>
+      <c r="B104" t="s">
+        <v>277</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104" t="s">
+        <v>277</v>
+      </c>
+      <c r="E104" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>222</v>
+      </c>
+      <c r="B105" t="s">
+        <v>227</v>
+      </c>
+      <c r="C105">
+        <v>2.62227608495596E-4</v>
+      </c>
+      <c r="D105" t="s">
+        <v>227</v>
+      </c>
+      <c r="E105" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>272</v>
+      </c>
+      <c r="B106" t="s">
+        <v>278</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106" t="s">
+        <v>278</v>
+      </c>
+      <c r="E106" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>119</v>
+      </c>
+      <c r="B107" t="s">
+        <v>130</v>
+      </c>
+      <c r="C107">
+        <v>5.0223820436918597E-4</v>
+      </c>
+      <c r="D107" t="s">
+        <v>130</v>
+      </c>
+      <c r="E107" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>288</v>
+      </c>
+      <c r="B108" t="s">
+        <v>288</v>
+      </c>
+      <c r="C108">
+        <v>1.4942570235631199E-3</v>
+      </c>
+      <c r="D108" t="s">
+        <v>174</v>
+      </c>
+      <c r="E108" s="24">
+        <v>0.6660287081339713</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>183</v>
+      </c>
+      <c r="B109" t="s">
+        <v>322</v>
+      </c>
+      <c r="C109" s="27">
+        <v>2.848860972467E-5</v>
+      </c>
+      <c r="E109" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110" t="s">
+        <v>313</v>
+      </c>
+      <c r="C110">
+        <v>1.04773018813506E-4</v>
+      </c>
+      <c r="D110" t="s">
+        <v>216</v>
+      </c>
+      <c r="E110" s="24">
+        <v>0.90341032957659839</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>236</v>
+      </c>
+      <c r="B111" t="s">
+        <v>302</v>
+      </c>
+      <c r="C111">
+        <v>1.64447937968658E-3</v>
+      </c>
+      <c r="D111" t="s">
+        <v>216</v>
+      </c>
+      <c r="E111" s="24">
+        <v>0.46153846153846156</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>257</v>
+      </c>
+      <c r="B112" t="s">
+        <v>316</v>
+      </c>
+      <c r="C112" s="27">
+        <v>4.6337151925198002E-5</v>
+      </c>
+      <c r="D112" t="s">
+        <v>216</v>
+      </c>
+      <c r="E112" s="24">
+        <v>0.46153846153846156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>172</v>
+      </c>
+      <c r="B113" t="s">
+        <v>178</v>
+      </c>
+      <c r="C113" s="27">
+        <v>4.3930321481960303E-5</v>
+      </c>
+      <c r="D113" t="s">
+        <v>178</v>
+      </c>
+      <c r="E113" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>272</v>
+      </c>
+      <c r="B114" t="s">
+        <v>279</v>
+      </c>
+      <c r="C114" s="27">
+        <v>3.4524285007145302E-5</v>
+      </c>
+      <c r="D114" t="s">
+        <v>279</v>
+      </c>
+      <c r="E114" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>291</v>
+      </c>
+      <c r="B115" t="s">
+        <v>296</v>
+      </c>
+      <c r="C115">
+        <v>9.8018242020467597E-4</v>
+      </c>
+      <c r="D115" t="s">
+        <v>296</v>
+      </c>
+      <c r="E115" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>342</v>
+      </c>
+      <c r="B116" t="s">
+        <v>181</v>
+      </c>
+      <c r="C116" s="27">
+        <v>5.9725825881480801E-6</v>
+      </c>
+      <c r="D116" t="s">
+        <v>181</v>
+      </c>
+      <c r="E116" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>236</v>
+      </c>
+      <c r="B117" t="s">
+        <v>243</v>
+      </c>
+      <c r="C117">
+        <v>3.0636495853791999E-3</v>
+      </c>
+      <c r="D117" t="s">
+        <v>243</v>
+      </c>
+      <c r="E117" s="24">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>